<commit_message>
aggiunto controllo su xls file in input
</commit_message>
<xml_diff>
--- a/toDoList.xlsx
+++ b/toDoList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Column6</t>
   </si>
@@ -448,7 +448,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,6 +515,9 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">

</xml_diff>